<commit_message>
Criação de todas sheets que precisam de testes
</commit_message>
<xml_diff>
--- a/Documentação/Planilha de UAT/Planilha de UAT.xlsx
+++ b/Documentação/Planilha de UAT/Planilha de UAT.xlsx
@@ -5,15 +5,24 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ghgoncalves\Desktop\project-hunter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a08d7f3c16d54179/Área de Trabalho/project-hunter/Documentação/Planilha de UAT/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BAB7EA99-D766-489B-9A41-15C1809A0F3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="8_{BAB7EA99-D766-489B-9A41-15C1809A0F3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{30C4AAA9-D588-4AA6-99FB-2D2CE4D0DACE}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{CCEB0146-9C4B-423C-9F76-223A38A39EE4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CCEB0146-9C4B-423C-9F76-223A38A39EE4}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
+    <sheet name="Continuação do Cadastro" sheetId="8" r:id="rId2"/>
+    <sheet name="Recuperação de Senha" sheetId="2" r:id="rId3"/>
+    <sheet name="Login" sheetId="3" r:id="rId4"/>
+    <sheet name="Home" sheetId="4" r:id="rId5"/>
+    <sheet name="Configurações" sheetId="5" r:id="rId6"/>
+    <sheet name="Perfil do Jogador" sheetId="6" r:id="rId7"/>
+    <sheet name="Perfil da Equipe" sheetId="7" r:id="rId8"/>
+    <sheet name="Buscar" sheetId="9" r:id="rId9"/>
+    <sheet name="Agendamento de Partida" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -153,11 +162,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,18 +485,18 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.28515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="56.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="56.6640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -497,8 +506,8 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="4"/>
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
@@ -506,8 +515,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
@@ -515,19 +524,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="4"/>
+      <c r="B5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -538,7 +547,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>2</v>
       </c>
@@ -549,7 +558,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -560,11 +569,11 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="2"/>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
@@ -574,8 +583,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
       <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
@@ -583,8 +592,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="4"/>
       <c r="B14" s="1" t="s">
         <v>4</v>
       </c>
@@ -592,19 +601,19 @@
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="4" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="4"/>
+      <c r="B16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>1</v>
       </c>
@@ -615,7 +624,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>2</v>
       </c>
@@ -626,7 +635,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>3</v>
       </c>
@@ -645,4 +654,114 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B56CACC0-D405-4DA8-B8A6-077CAD7A68D7}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CD546F0-FDFF-4749-99C1-D833D04C885B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E80CEFA5-6735-4CD9-AC59-D924DA2618BB}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEF6AEAB-FBF6-43E5-8942-7553830315CA}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E121097-8404-41AE-9FE2-0519B88B3910}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74B472FB-5909-4047-9318-E6AD5E5B4018}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F83F4D-E66C-40FF-8308-FE5308B374E1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D53305D5-B540-4BFE-BA81-2DFA2BF408E0}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CAA44DC-3DD9-4458-9AA3-B8D422510AB8}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>